<commit_message>
Latest Update_Up to Model building
</commit_message>
<xml_diff>
--- a/Fatigue database of High-entropy alloys.xlsx
+++ b/Fatigue database of High-entropy alloys.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihle\Python_programs\Own_Projects\Material_Performance_n_Failure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mihle\Python_programs\Own_Projects\Material_Performance_and_Failure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE752C2E-5D9A-4ECA-A3BA-F8BE28FD86C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86C9136D-FC7E-41A0-8414-1D730A8F7510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="809" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1053" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1051" uniqueCount="341">
   <si>
     <t>ID</t>
   </si>
@@ -298,9 +298,6 @@
   </si>
   <si>
     <t>250–500</t>
-  </si>
-  <si>
-    <t>123-132</t>
   </si>
   <si>
     <t>Kashaev, N., Ventzke, V., Petrov, N., Horstmann, M., Zherebtsov, S., Shaysultanov, D., Sanin, V. and Stepanov, N., 2019. Fatigue behaviour of a laser beam welded CoCrFeNiMn-type high entropy alloy. Materials Science and Engineering: A, 766, p.138358.</t>
@@ -914,10 +911,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>CoCrFeMnNi</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Fe50Mn30Co10Cr10</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -1129,10 +1122,6 @@
   </si>
   <si>
     <t>Dendritic FCC + interdendritic FCC</t>
-  </si>
-  <si>
-    <t>Al0.5CoCrFeNi</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Al0.5CoCrCuFeNi</t>
@@ -1309,6 +1298,12 @@
       </rPr>
       <t>, 1–43. https://doi.org/10.2139/ssrn.3708757</t>
     </r>
+  </si>
+  <si>
+    <t>Fe50Mn30Co10Cr10</t>
+  </si>
+  <si>
+    <t>Al0.5CoCrFeNi</t>
   </si>
 </sst>
 </file>
@@ -1855,103 +1850,103 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" customHeight="1">
       <c r="A1" s="46" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="13.8">
       <c r="A2" s="48" t="s">
+        <v>250</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>251</v>
-      </c>
-      <c r="B2" s="48" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="13.8">
       <c r="A3" s="48" t="s">
+        <v>252</v>
+      </c>
+      <c r="B3" s="48" t="s">
         <v>253</v>
-      </c>
-      <c r="B3" s="48" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="13.8">
       <c r="A4" s="48" t="s">
+        <v>254</v>
+      </c>
+      <c r="B4" s="48" t="s">
         <v>255</v>
-      </c>
-      <c r="B4" s="48" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="13.8">
       <c r="A5" s="48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" customHeight="1">
       <c r="A6" s="48" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" customHeight="1">
       <c r="A7" s="48" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" customHeight="1">
       <c r="A8" s="48" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B8" s="48" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" customHeight="1">
       <c r="A9" s="48" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15" customHeight="1">
       <c r="A10" s="48" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15" customHeight="1">
       <c r="A11" s="48" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="B11" s="48" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15" customHeight="1">
       <c r="A12" s="48" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15" customHeight="1">
       <c r="A13" s="48" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -2948,8 +2943,8 @@
   </sheetPr>
   <dimension ref="A1:Q996"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -2987,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -3002,7 +2997,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -3026,7 +3021,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="13.8">
@@ -3034,7 +3029,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>260</v>
+        <v>24</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>18</v>
@@ -3071,7 +3066,7 @@
         <v>21</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>22</v>
@@ -3080,7 +3075,7 @@
         <v>23</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="13.8">
@@ -3091,7 +3086,7 @@
         <v>24</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>25</v>
@@ -3180,10 +3175,10 @@
         <v>26</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>31</v>
@@ -3233,7 +3228,7 @@
         <v>34</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>35</v>
@@ -3247,7 +3242,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>37</v>
@@ -3286,13 +3281,13 @@
         <v>34</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>38</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="7" spans="1:17" ht="13.8">
@@ -3300,7 +3295,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>39</v>
@@ -3339,13 +3334,13 @@
         <v>34</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>38</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="8" spans="1:17" ht="13.8">
@@ -3353,7 +3348,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>40</v>
@@ -3392,13 +3387,13 @@
         <v>34</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="9" spans="1:17" ht="13.8">
@@ -3406,7 +3401,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>41</v>
@@ -3445,13 +3440,13 @@
         <v>34</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="P9" s="3" t="s">
         <v>38</v>
       </c>
       <c r="Q9" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:17" ht="13.8">
@@ -3498,13 +3493,13 @@
         <v>34</v>
       </c>
       <c r="O10" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="P10" s="3" t="s">
         <v>45</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="13.8">
@@ -3551,13 +3546,13 @@
         <v>34</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="P11" s="3" t="s">
         <v>45</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:17" ht="13.8">
@@ -3565,7 +3560,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>261</v>
+        <v>339</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>47</v>
@@ -3604,13 +3599,13 @@
         <v>34</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="P12" s="3" t="s">
         <v>49</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="13.8">
@@ -3618,7 +3613,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>50</v>
@@ -3657,13 +3652,13 @@
         <v>34</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="P13" s="3" t="s">
         <v>49</v>
       </c>
       <c r="Q13" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:17" ht="13.8">
@@ -3671,13 +3666,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>319</v>
+        <v>340</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E14" s="3">
         <v>9</v>
@@ -3701,22 +3696,22 @@
         <v>-1</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M14" s="3" t="s">
         <v>21</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O14" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="P14" s="11" t="s">
         <v>213</v>
       </c>
-      <c r="P14" s="11" t="s">
-        <v>214</v>
-      </c>
       <c r="Q14" s="12" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="15" spans="1:17" ht="13.8" customHeight="1">
@@ -3727,25 +3722,25 @@
         <v>24</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E15" s="3">
         <v>60</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J15" s="3">
         <v>298</v>
@@ -3754,22 +3749,22 @@
         <v>-1</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M15" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="N15" s="3" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="O15" s="3" t="s">
         <v>22</v>
       </c>
       <c r="P15" s="11" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="Q15" s="12" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:17" ht="13.8"/>
@@ -4791,16 +4786,16 @@
         <v>16</v>
       </c>
       <c r="C1" s="42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D1" s="42" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="42" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F1" s="42" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.8">
@@ -7601,8 +7596,8 @@
   </sheetPr>
   <dimension ref="A1:V996"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L24"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L26" sqref="L26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1"/>
@@ -7644,7 +7639,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>3</v>
@@ -7659,7 +7654,7 @@
         <v>56</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>7</v>
@@ -7706,10 +7701,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>65</v>
@@ -7745,10 +7740,10 @@
         <v>20</v>
       </c>
       <c r="O2" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>306</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>308</v>
       </c>
       <c r="Q2" s="5">
         <v>383</v>
@@ -7766,7 +7761,7 @@
         <v>42292</v>
       </c>
       <c r="V2" s="10" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="13.8">
@@ -7774,10 +7769,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>68</v>
@@ -7813,10 +7808,10 @@
         <v>20</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Q3" s="5">
         <v>380</v>
@@ -7842,10 +7837,10 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>68</v>
@@ -7881,10 +7876,10 @@
         <v>20</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P4" s="5" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="Q4" s="5">
         <v>470</v>
@@ -7949,7 +7944,7 @@
         <v>20</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P5" s="5" t="s">
         <v>20</v>
@@ -8017,7 +8012,7 @@
         <v>20</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P6" s="5" t="s">
         <v>20</v>
@@ -8049,7 +8044,7 @@
         <v>74</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>75</v>
@@ -8085,10 +8080,10 @@
         <v>20</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="Q7" s="5">
         <v>456</v>
@@ -8114,10 +8109,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>77</v>
@@ -8153,7 +8148,7 @@
         <v>20</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P8" s="5" t="s">
         <v>20</v>
@@ -8182,10 +8177,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>79</v>
@@ -8221,7 +8216,7 @@
         <v>20</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P9" s="5" t="s">
         <v>20</v>
@@ -8250,10 +8245,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>81</v>
@@ -8289,7 +8284,7 @@
         <v>20</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="P10" s="5" t="s">
         <v>20</v>
@@ -8321,7 +8316,7 @@
         <v>82</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>25</v>
@@ -8357,10 +8352,10 @@
         <v>20</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P11" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q11" s="5">
         <v>495</v>
@@ -8389,7 +8384,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>25</v>
@@ -8425,10 +8420,10 @@
         <v>20</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P12" s="5" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="Q12" s="5">
         <v>450</v>
@@ -8457,7 +8452,7 @@
         <v>82</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>25</v>
@@ -8493,10 +8488,10 @@
         <v>20</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Q13" s="5">
         <v>280</v>
@@ -8525,7 +8520,7 @@
         <v>82</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>25</v>
@@ -8561,10 +8556,10 @@
         <v>20</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P14" s="5" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="Q14" s="5">
         <v>190</v>
@@ -8593,7 +8588,7 @@
         <v>82</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>25</v>
@@ -8623,16 +8618,16 @@
         <v>30</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="N15" s="5" t="s">
         <v>20</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P15" s="5" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="Q15" s="5">
         <v>250</v>
@@ -8650,7 +8645,7 @@
         <v>43802</v>
       </c>
       <c r="V15" s="10" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="13.8">
@@ -8687,8 +8682,8 @@
       <c r="K16" s="5">
         <v>0.1</v>
       </c>
-      <c r="L16" s="5" t="s">
-        <v>87</v>
+      <c r="L16" s="5">
+        <v>123</v>
       </c>
       <c r="M16" s="5" t="s">
         <v>21</v>
@@ -8697,10 +8692,10 @@
         <v>20</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P16" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Q16" s="5">
         <v>90</v>
@@ -8718,7 +8713,7 @@
         <v>43707</v>
       </c>
       <c r="V16" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="13.8">
@@ -8729,13 +8724,13 @@
         <v>82</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F17" s="5">
         <v>164</v>
@@ -8755,8 +8750,8 @@
       <c r="K17" s="5">
         <v>0.1</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>87</v>
+      <c r="L17" s="5">
+        <v>123</v>
       </c>
       <c r="M17" s="5" t="s">
         <v>21</v>
@@ -8765,10 +8760,10 @@
         <v>20</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P17" s="5" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="Q17" s="5">
         <v>90</v>
@@ -8786,7 +8781,7 @@
         <v>43707</v>
       </c>
       <c r="V17" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="13.8">
@@ -8797,7 +8792,7 @@
         <v>82</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>25</v>
@@ -8833,10 +8828,10 @@
         <v>20</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P18" s="5" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="Q18" s="5">
         <v>126</v>
@@ -8854,7 +8849,7 @@
         <v>43581</v>
       </c>
       <c r="V18" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="13.8">
@@ -8865,13 +8860,13 @@
         <v>82</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F19" s="5">
         <v>851.2</v>
@@ -8895,16 +8890,16 @@
         <v>50</v>
       </c>
       <c r="M19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="N19" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="N19" s="5" t="s">
+      <c r="O19" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="P19" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="P19" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="Q19" s="5">
         <v>549</v>
@@ -8922,7 +8917,7 @@
         <v>43990</v>
       </c>
       <c r="V19" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="13.8">
@@ -8933,13 +8928,13 @@
         <v>82</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F20" s="5">
         <v>770.1</v>
@@ -8954,7 +8949,7 @@
         <v>0.23</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K20" s="5">
         <v>-1</v>
@@ -8963,16 +8958,16 @@
         <v>50</v>
       </c>
       <c r="M20" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="N20" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="O20" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="P20" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="O20" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="P20" s="5" t="s">
-        <v>146</v>
       </c>
       <c r="Q20" s="5">
         <v>474</v>
@@ -8990,7 +8985,7 @@
         <v>43991</v>
       </c>
       <c r="V20" s="5" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1">
@@ -9001,7 +8996,7 @@
         <v>24</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>25</v>
@@ -9022,7 +9017,7 @@
         <v>0.63</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K21" s="5">
         <v>-1</v>
@@ -9031,16 +9026,16 @@
         <v>20000</v>
       </c>
       <c r="M21" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="N21" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="O21" s="5" t="s">
-        <v>217</v>
-      </c>
       <c r="P21" s="5" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="Q21" s="5">
         <v>230</v>
@@ -9055,10 +9050,10 @@
         <v>0.35</v>
       </c>
       <c r="U21" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="V21" s="5" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="15.75" customHeight="1">
@@ -9069,10 +9064,10 @@
         <v>24</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E22" s="5">
         <v>10</v>
@@ -9084,13 +9079,13 @@
         <v>923</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I22" s="5">
         <v>0.308</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K22" s="5">
         <v>0.1</v>
@@ -9099,16 +9094,16 @@
         <v>20</v>
       </c>
       <c r="M22" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="N22" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="N22" s="5" t="s">
-        <v>221</v>
-      </c>
       <c r="O22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="P22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q22" s="5">
         <v>257</v>
@@ -9123,10 +9118,10 @@
         <v>0.27800000000000002</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V22" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="15.75" customHeight="1">
@@ -9134,16 +9129,16 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F23" s="5">
         <v>1284</v>
@@ -9152,13 +9147,13 @@
         <v>1344</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J23" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K23" s="5">
         <v>0.1</v>
@@ -9167,16 +9162,16 @@
         <v>10</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q23" s="5">
         <v>363</v>
@@ -9191,10 +9186,10 @@
         <v>0.28999999999999998</v>
       </c>
       <c r="U23" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="V23" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="15.75" customHeight="1">
@@ -9205,10 +9200,10 @@
         <v>74</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E24" s="5">
         <v>45</v>
@@ -9220,13 +9215,13 @@
         <v>1139</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I24" s="5">
         <v>0.16</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K24" s="5">
         <v>0.1</v>
@@ -9235,16 +9230,16 @@
         <v>10</v>
       </c>
       <c r="M24" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="O24" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="Q24" s="5">
         <v>512</v>
@@ -9259,10 +9254,10 @@
         <v>0.45</v>
       </c>
       <c r="U24" s="5" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="V24" s="5" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
     </row>
     <row r="25" spans="1:22" ht="15.75" customHeight="1"/>
@@ -17173,7 +17168,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -17188,7 +17183,7 @@
         <v>6</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>7</v>
@@ -17209,13 +17204,13 @@
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>96</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>97</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>15</v>
@@ -17226,10 +17221,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>99</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>100</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>25</v>
@@ -17256,28 +17251,28 @@
         <v>0.1</v>
       </c>
       <c r="L2" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="N2" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q2" s="5">
         <v>6.2</v>
       </c>
       <c r="R2" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="S2" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="13.8">
@@ -17285,10 +17280,10 @@
         <v>2</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>25</v>
@@ -17315,28 +17310,28 @@
         <v>0.1</v>
       </c>
       <c r="L3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="M3" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="N3" s="5" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q3" s="5">
         <v>7.4</v>
       </c>
       <c r="R3" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="S3" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="S3" s="5" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="13.8">
@@ -17347,7 +17342,7 @@
         <v>74</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>75</v>
@@ -17374,16 +17369,16 @@
         <v>0.1</v>
       </c>
       <c r="L4" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="M4" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="M4" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="N4" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O4" s="5" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="P4" s="5">
         <v>2.5</v>
@@ -17392,10 +17387,10 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="R4" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="S4" s="12" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="13.8">
@@ -17403,16 +17398,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F5" s="5">
         <v>410</v>
@@ -17433,16 +17428,16 @@
         <v>0.1</v>
       </c>
       <c r="L5" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M5" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N5" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P5" s="5">
         <v>4.8</v>
@@ -17451,10 +17446,10 @@
         <v>3.5</v>
       </c>
       <c r="R5" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S5" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="13.8">
@@ -17462,16 +17457,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F6" s="5">
         <v>520</v>
@@ -17492,16 +17487,16 @@
         <v>0.1</v>
       </c>
       <c r="L6" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M6" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M6" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N6" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P6" s="5">
         <v>6.3</v>
@@ -17510,10 +17505,10 @@
         <v>4.5</v>
       </c>
       <c r="R6" s="5" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S6" s="12" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="13.8">
@@ -17521,28 +17516,28 @@
         <v>6</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J7" s="5">
         <v>77</v>
@@ -17551,28 +17546,28 @@
         <v>0.1</v>
       </c>
       <c r="L7" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M7" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N7" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q7" s="5">
         <v>2.9</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S7" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="13.8">
@@ -17580,28 +17575,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I8" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J8" s="5">
         <v>293</v>
@@ -17610,16 +17605,16 @@
         <v>0.4</v>
       </c>
       <c r="L8" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M8" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M8" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N8" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P8" s="5">
         <v>2.6</v>
@@ -17628,10 +17623,10 @@
         <v>2.8</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S8" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="13.8">
@@ -17639,28 +17634,28 @@
         <v>8</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J9" s="5">
         <v>198</v>
@@ -17669,16 +17664,16 @@
         <v>0.4</v>
       </c>
       <c r="L9" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M9" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M9" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N9" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O9" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P9" s="5">
         <v>4.8</v>
@@ -17687,10 +17682,10 @@
         <v>3.4</v>
       </c>
       <c r="R9" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S9" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="13.8">
@@ -17698,28 +17693,28 @@
         <v>9</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J10" s="5">
         <v>77</v>
@@ -17728,28 +17723,28 @@
         <v>0.4</v>
       </c>
       <c r="L10" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M10" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M10" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N10" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="P10" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q10" s="5">
         <v>2.2999999999999998</v>
       </c>
       <c r="R10" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S10" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="13.8">
@@ -17757,28 +17752,28 @@
         <v>10</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I11" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J11" s="5">
         <v>293</v>
@@ -17787,16 +17782,16 @@
         <v>0.7</v>
       </c>
       <c r="L11" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M11" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M11" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N11" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O11" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P11" s="5">
         <v>2.5</v>
@@ -17805,10 +17800,10 @@
         <v>2.6</v>
       </c>
       <c r="R11" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S11" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="13.8">
@@ -17816,28 +17811,28 @@
         <v>11</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C12" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J12" s="5">
         <v>198</v>
@@ -17846,16 +17841,16 @@
         <v>0.7</v>
       </c>
       <c r="L12" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M12" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M12" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N12" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O12" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P12" s="5">
         <v>3.5</v>
@@ -17864,10 +17859,10 @@
         <v>3.1</v>
       </c>
       <c r="R12" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S12" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="13.8">
@@ -17875,28 +17870,28 @@
         <v>12</v>
       </c>
       <c r="B13" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J13" s="5">
         <v>77</v>
@@ -17905,28 +17900,28 @@
         <v>0.7</v>
       </c>
       <c r="L13" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M13" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="M13" s="5" t="s">
-        <v>113</v>
-      </c>
       <c r="N13" s="5" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="P13" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q13" s="5">
         <v>2.2999999999999998</v>
       </c>
       <c r="R13" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S13" s="12" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="13.8">
@@ -17934,13 +17929,13 @@
         <v>13</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>20</v>
@@ -17964,16 +17959,16 @@
         <v>0.1</v>
       </c>
       <c r="L14" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M14" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P14" s="5">
         <v>17</v>
@@ -17982,10 +17977,10 @@
         <v>3.4</v>
       </c>
       <c r="R14" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S14" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:19" ht="13.8">
@@ -17993,13 +17988,13 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>20</v>
@@ -18023,16 +18018,16 @@
         <v>0.3</v>
       </c>
       <c r="L15" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P15" s="5">
         <v>5</v>
@@ -18041,10 +18036,10 @@
         <v>6.5</v>
       </c>
       <c r="R15" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S15" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:19" ht="13.8">
@@ -18052,13 +18047,13 @@
         <v>15</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C16" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>20</v>
@@ -18082,16 +18077,16 @@
         <v>0.7</v>
       </c>
       <c r="L16" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P16" s="5">
         <v>7</v>
@@ -18100,10 +18095,10 @@
         <v>14.5</v>
       </c>
       <c r="R16" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S16" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="17" spans="1:19" ht="13.8">
@@ -18111,13 +18106,13 @@
         <v>16</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C17" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D17" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E17" s="5" t="s">
         <v>20</v>
@@ -18141,16 +18136,16 @@
         <v>0.1</v>
       </c>
       <c r="L17" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M17" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N17" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P17" s="5">
         <v>16</v>
@@ -18159,10 +18154,10 @@
         <v>4.9000000000000004</v>
       </c>
       <c r="R17" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S17" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:19" ht="13.8">
@@ -18170,13 +18165,13 @@
         <v>17</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C18" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D18" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E18" s="5" t="s">
         <v>20</v>
@@ -18200,16 +18195,16 @@
         <v>0.3</v>
       </c>
       <c r="L18" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M18" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N18" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P18" s="5">
         <v>7</v>
@@ -18218,10 +18213,10 @@
         <v>5.3</v>
       </c>
       <c r="R18" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S18" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="13.8">
@@ -18229,13 +18224,13 @@
         <v>18</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C19" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="E19" s="5" t="s">
         <v>20</v>
@@ -18259,16 +18254,16 @@
         <v>0.7</v>
       </c>
       <c r="L19" s="5" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="N19" s="5" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="P19" s="5">
         <v>5</v>
@@ -18277,10 +18272,10 @@
         <v>25.8</v>
       </c>
       <c r="R19" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="S19" s="12" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="15.75" customHeight="1">
@@ -18288,16 +18283,16 @@
         <v>19</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="D20" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="E20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F20" s="5">
         <v>172</v>
@@ -18321,25 +18316,25 @@
         <v>33</v>
       </c>
       <c r="M20" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N20" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="N20" s="5" t="s">
+      <c r="O20" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="O20" s="5" t="s">
-        <v>124</v>
-      </c>
       <c r="P20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q20" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R20" s="5">
         <v>12.2018</v>
       </c>
       <c r="S20" s="12" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="15.75" customHeight="1">
@@ -18347,28 +18342,28 @@
         <v>20</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="E21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J21" s="5">
         <v>373</v>
@@ -18377,28 +18372,28 @@
         <v>0.1</v>
       </c>
       <c r="L21" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="M21" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N21" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O21" s="5" t="s">
         <v>200</v>
       </c>
-      <c r="M21" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="N21" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="O21" s="5" t="s">
+      <c r="P21" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="Q21" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="R21" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="P21" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="Q21" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="R21" s="5" t="s">
-        <v>202</v>
-      </c>
       <c r="S21" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:19" ht="15.75" customHeight="1">
@@ -18406,28 +18401,28 @@
         <v>21</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="D22" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="E22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J22" s="5">
         <v>298</v>
@@ -18436,28 +18431,28 @@
         <v>0.1</v>
       </c>
       <c r="L22" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="M22" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="O22" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="M22" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="N22" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="O22" s="5" t="s">
-        <v>204</v>
-      </c>
       <c r="P22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S22" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:19" ht="15.75" customHeight="1">
@@ -18465,28 +18460,28 @@
         <v>22</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="E23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J23" s="5">
         <v>198</v>
@@ -18495,28 +18490,28 @@
         <v>0.1</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M23" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N23" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="N23" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="O23" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="P23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q23" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R23" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S23" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="24" spans="1:19" ht="15.75" customHeight="1">
@@ -18524,28 +18519,28 @@
         <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="D24" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>121</v>
-      </c>
       <c r="E24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J24" s="5">
         <v>103</v>
@@ -18554,28 +18549,28 @@
         <v>0.1</v>
       </c>
       <c r="L24" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="M24" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="N24" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="N24" s="5" t="s">
-        <v>123</v>
-      </c>
       <c r="O24" s="5" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="P24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q24" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R24" s="5" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="S24" s="12" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:19" ht="15.75" customHeight="1">
@@ -18583,10 +18578,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>25</v>
@@ -18616,13 +18611,13 @@
         <v>33</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N25" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P25" s="5">
         <v>5.5</v>
@@ -18631,10 +18626,10 @@
         <v>3.21</v>
       </c>
       <c r="R25" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="S25" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:19" ht="15.75" customHeight="1">
@@ -18642,10 +18637,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>25</v>
@@ -18675,13 +18670,13 @@
         <v>33</v>
       </c>
       <c r="M26" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="N26" s="5" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P26" s="5">
         <v>5.5</v>
@@ -18690,10 +18685,10 @@
         <v>2.5099999999999998</v>
       </c>
       <c r="R26" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S26" s="12" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="27" spans="1:19" ht="15.75" customHeight="1">
@@ -18704,7 +18699,7 @@
         <v>24</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D27" s="14" t="s">
         <v>25</v>
@@ -18713,16 +18708,16 @@
         <v>20</v>
       </c>
       <c r="F27" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G27" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J27" s="14">
         <v>298</v>
@@ -18731,28 +18726,28 @@
         <v>0.1</v>
       </c>
       <c r="L27" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M27" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="N27" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="N27" s="14" t="s">
-        <v>123</v>
-      </c>
       <c r="O27" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="P27" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q27" s="14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="R27" s="14">
         <v>10.202</v>
       </c>
       <c r="S27" s="16" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="28" spans="1:19" ht="15.75" customHeight="1">
@@ -18760,28 +18755,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D28" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J28" s="5">
         <v>298</v>
@@ -18790,28 +18785,28 @@
         <v>0.05</v>
       </c>
       <c r="L28" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="M28" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M28" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="N28" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O28" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P28" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q28" s="5">
         <v>2.5499999999999998</v>
       </c>
       <c r="R28" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="S28" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="29" spans="1:19" ht="15.75" customHeight="1">
@@ -18819,28 +18814,28 @@
         <v>28</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D29" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>208</v>
       </c>
       <c r="E29" s="5" t="s">
         <v>20</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="I29" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="J29" s="5">
         <v>298</v>
@@ -18849,28 +18844,28 @@
         <v>0.2</v>
       </c>
       <c r="L29" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="M29" s="5" t="s">
         <v>209</v>
       </c>
-      <c r="M29" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="N29" s="5" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="O29" s="5" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="P29" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="Q29" s="5">
         <v>2.29</v>
       </c>
       <c r="R29" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="S29" s="12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="30" spans="1:19" ht="15.75" customHeight="1"/>
@@ -19978,261 +19973,261 @@
   <sheetData>
     <row r="1" spans="1:111" s="23" customFormat="1" ht="13.8">
       <c r="A1" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="21" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>93</v>
-      </c>
       <c r="F1" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G1" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="I1" s="21" t="s">
         <v>52</v>
       </c>
       <c r="J1" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K1" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="M1" s="21" t="s">
         <v>53</v>
       </c>
       <c r="N1" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="O1" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="Q1" s="21" t="s">
         <v>55</v>
       </c>
       <c r="R1" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="S1" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="U1" s="21" t="s">
+        <v>150</v>
+      </c>
+      <c r="V1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="W1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="Y1" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="V1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="W1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="Y1" s="24" t="s">
+      <c r="Z1" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="AA1" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="AC1" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="Z1" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="AA1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="AE1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="AG1" s="21" t="s">
         <v>153</v>
       </c>
-      <c r="AD1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="AE1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="AG1" s="21" t="s">
+      <c r="AH1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AI1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="AK1" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="AH1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="AI1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="AK1" s="25" t="s">
+      <c r="AL1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="AM1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="AO1" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="AL1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="AM1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="AO1" s="25" t="s">
+      <c r="AP1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="AQ1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="AS1" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="AP1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="AQ1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="AS1" s="25" t="s">
+      <c r="AT1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="AU1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="AW1" s="21" t="s">
         <v>157</v>
       </c>
-      <c r="AT1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="AU1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="AW1" s="21" t="s">
+      <c r="AX1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="AY1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="BA1" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="AX1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="AY1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="BA1" s="25" t="s">
+      <c r="BB1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="BC1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="BE1" s="21" t="s">
         <v>159</v>
       </c>
-      <c r="BB1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="BE1" s="21" t="s">
+      <c r="BF1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="BG1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="BI1" s="21" t="s">
         <v>160</v>
       </c>
-      <c r="BF1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="BG1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="BI1" s="21" t="s">
+      <c r="BJ1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="BK1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="BM1" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="BJ1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="BK1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="BM1" s="25" t="s">
+      <c r="BN1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="BO1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="BQ1" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="BN1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="BO1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="BQ1" s="25" t="s">
+      <c r="BR1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="BS1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="BU1" s="21" t="s">
         <v>163</v>
       </c>
-      <c r="BR1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="BS1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="BU1" s="21" t="s">
+      <c r="BV1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="BW1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="BY1" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="BV1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="BW1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="BY1" s="25" t="s">
+      <c r="BZ1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="CA1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="CC1" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="BZ1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="CA1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="CC1" s="25" t="s">
+      <c r="CD1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="CE1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="CG1" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="CD1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="CE1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="CG1" s="25" t="s">
+      <c r="CH1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="CI1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="CK1" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="CH1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="CI1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="CK1" s="24" t="s">
+      <c r="CL1" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="CM1" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="CO1" s="21" t="s">
         <v>168</v>
       </c>
-      <c r="CL1" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="CM1" s="24" t="s">
-        <v>131</v>
-      </c>
-      <c r="CO1" s="21" t="s">
+      <c r="CP1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="CQ1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="CS1" s="21" t="s">
         <v>169</v>
       </c>
-      <c r="CP1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="CQ1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="CS1" s="21" t="s">
+      <c r="CT1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="CU1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="CW1" s="21" t="s">
         <v>170</v>
       </c>
-      <c r="CT1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="CU1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="CW1" s="21" t="s">
+      <c r="CX1" s="21" t="s">
+        <v>97</v>
+      </c>
+      <c r="CY1" s="21" t="s">
+        <v>130</v>
+      </c>
+      <c r="DA1" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="CX1" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="CY1" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="DA1" s="25" t="s">
+      <c r="DB1" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="DC1" s="25" t="s">
+        <v>130</v>
+      </c>
+      <c r="DE1" s="21" t="s">
         <v>172</v>
       </c>
-      <c r="DB1" s="25" t="s">
-        <v>98</v>
-      </c>
-      <c r="DC1" s="25" t="s">
-        <v>131</v>
-      </c>
-      <c r="DE1" s="21" t="s">
-        <v>173</v>
-      </c>
       <c r="DF1" s="25" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="DG1" s="25" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:111" ht="13.8">
       <c r="A2" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B2" s="18">
         <v>14.56972987</v>
@@ -20241,7 +20236,7 @@
         <v>1.96E-8</v>
       </c>
       <c r="E2" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F2" s="18">
         <v>18.09688594</v>
@@ -20259,7 +20254,7 @@
         <v>3.5400000000000002E-9</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N2" s="18">
         <v>4.9175132069999998</v>
@@ -20269,7 +20264,7 @@
       </c>
       <c r="P2" s="27"/>
       <c r="Q2" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="R2" s="18">
         <v>6.1866650410000004</v>
@@ -20279,7 +20274,7 @@
       </c>
       <c r="T2" s="27"/>
       <c r="U2" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="V2" s="18">
         <v>8.8478553998472407</v>
@@ -20289,7 +20284,7 @@
       </c>
       <c r="X2" s="27"/>
       <c r="Y2" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="Z2" s="28">
         <v>2.5381900000000002</v>
@@ -20299,7 +20294,7 @@
       </c>
       <c r="AB2" s="27"/>
       <c r="AC2" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AD2" s="28">
         <v>4.8201599999999996</v>
@@ -20309,7 +20304,7 @@
       </c>
       <c r="AF2" s="27"/>
       <c r="AG2" s="18" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AH2" s="18">
         <v>5.0513322681142201</v>
@@ -20318,7 +20313,7 @@
         <v>7.2376657462354599E-10</v>
       </c>
       <c r="AK2" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="AL2" s="28">
         <v>2.4309799999999999</v>
@@ -20328,7 +20323,7 @@
       </c>
       <c r="AN2" s="27"/>
       <c r="AO2" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AP2" s="28">
         <v>3.4338099999999998</v>
@@ -20338,7 +20333,7 @@
       </c>
       <c r="AR2" s="27"/>
       <c r="AS2" s="28" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AT2" s="28">
         <v>4.8452540395660897</v>
@@ -20347,7 +20342,7 @@
         <v>7.0118548221599904E-10</v>
       </c>
       <c r="AW2" s="18" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AX2" s="18">
         <v>15.130554679999999</v>
@@ -20356,7 +20351,7 @@
         <v>6.4900000000000003E-10</v>
       </c>
       <c r="BA2" s="28" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BB2" s="28">
         <v>5.3651099999999996</v>
@@ -20366,7 +20361,7 @@
       </c>
       <c r="BD2" s="27"/>
       <c r="BE2" s="30" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="BF2" s="28">
         <v>7.1245000000000003</v>
@@ -20376,7 +20371,7 @@
       </c>
       <c r="BH2" s="27"/>
       <c r="BI2" s="18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BJ2" s="18">
         <v>13.898966400000001</v>
@@ -20385,7 +20380,7 @@
         <v>4.8200000000000005E-11</v>
       </c>
       <c r="BM2" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BN2" s="28">
         <v>7.21089</v>
@@ -20395,7 +20390,7 @@
       </c>
       <c r="BP2" s="27"/>
       <c r="BQ2" s="28" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="BR2" s="28">
         <v>5.07768</v>
@@ -20414,7 +20409,7 @@
         <v>2.4599999999999999E-8</v>
       </c>
       <c r="BY2" s="28" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BZ2" s="28">
         <v>15.899459999999999</v>
@@ -20424,7 +20419,7 @@
       </c>
       <c r="CB2" s="27"/>
       <c r="CC2" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="CD2" s="28">
         <v>14.9477743328915</v>
@@ -20433,7 +20428,7 @@
         <v>1.9345380572484E-8</v>
       </c>
       <c r="CG2" s="28" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="CH2" s="28">
         <v>16.247</v>
@@ -20443,7 +20438,7 @@
       </c>
       <c r="CJ2" s="27"/>
       <c r="CK2" s="28" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="CL2" s="28">
         <v>16.014469999999999</v>
@@ -20480,7 +20475,7 @@
         <v>1.1292799999999999E-7</v>
       </c>
       <c r="DA2" s="28" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="DB2" s="28">
         <v>7.5813199999999998</v>
@@ -20490,7 +20485,7 @@
       </c>
       <c r="DD2" s="27"/>
       <c r="DE2" s="30" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="DF2" s="28">
         <v>9.4868299999999994</v>
@@ -20501,7 +20496,7 @@
     </row>
     <row r="3" spans="1:111" ht="13.8">
       <c r="A3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B3" s="18">
         <v>14.34515109</v>
@@ -20510,7 +20505,7 @@
         <v>2.5299999999999998E-8</v>
       </c>
       <c r="E3" s="18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F3" s="18">
         <v>19.796946689999999</v>
@@ -20519,7 +20514,7 @@
         <v>1.3000000000000001E-8</v>
       </c>
       <c r="I3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J3" s="18">
         <v>2.8570557280000002</v>
@@ -20528,7 +20523,7 @@
         <v>6.2500000000000005E-9</v>
       </c>
       <c r="M3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N3" s="18">
         <v>4.8748077390000004</v>
@@ -20538,7 +20533,7 @@
       </c>
       <c r="P3" s="27"/>
       <c r="Q3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="R3" s="18">
         <v>6.2146919379999996</v>
@@ -20548,7 +20543,7 @@
       </c>
       <c r="T3" s="27"/>
       <c r="U3" s="18" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V3" s="18">
         <v>9.11957214630268</v>
@@ -20558,7 +20553,7 @@
       </c>
       <c r="X3" s="27"/>
       <c r="Y3" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="Z3" s="28">
         <v>2.5524</v>
@@ -20568,7 +20563,7 @@
       </c>
       <c r="AB3" s="27"/>
       <c r="AC3" s="28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AD3" s="28">
         <v>4.7263200000000003</v>
@@ -20578,7 +20573,7 @@
       </c>
       <c r="AF3" s="27"/>
       <c r="AG3" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AH3" s="18">
         <v>5.2660096589604901</v>
@@ -20587,7 +20582,7 @@
         <v>8.2208256916946402E-10</v>
       </c>
       <c r="AK3" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AL3" s="28">
         <v>2.53891</v>
@@ -20597,7 +20592,7 @@
       </c>
       <c r="AN3" s="27"/>
       <c r="AO3" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AP3" s="28">
         <v>3.4507300000000001</v>
@@ -20607,7 +20602,7 @@
       </c>
       <c r="AR3" s="27"/>
       <c r="AS3" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AT3" s="28">
         <v>4.97532855245628</v>
@@ -20616,7 +20611,7 @@
         <v>7.4727388735161801E-10</v>
       </c>
       <c r="AW3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AX3" s="18">
         <v>15.805295839999999</v>
@@ -20625,7 +20620,7 @@
         <v>8.1199999999999999E-10</v>
       </c>
       <c r="BA3" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BB3" s="28">
         <v>5.4042700000000004</v>
@@ -20635,7 +20630,7 @@
       </c>
       <c r="BD3" s="27"/>
       <c r="BE3" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BF3" s="28">
         <v>7.1245000000000003</v>
@@ -20645,7 +20640,7 @@
       </c>
       <c r="BH3" s="27"/>
       <c r="BI3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BJ3" s="18">
         <v>13.73929965</v>
@@ -20654,7 +20649,7 @@
         <v>7.4099999999999995E-11</v>
       </c>
       <c r="BM3" s="28" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="BN3" s="28">
         <v>7.3674099999999996</v>
@@ -20664,7 +20659,7 @@
       </c>
       <c r="BP3" s="27"/>
       <c r="BQ3" s="28" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="BR3" s="28">
         <v>5.0414599999999998</v>
@@ -20674,7 +20669,7 @@
       </c>
       <c r="BT3" s="27"/>
       <c r="BU3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="BV3" s="18">
         <v>16.498522269999999</v>
@@ -20683,7 +20678,7 @@
         <v>3.0099999999999998E-8</v>
       </c>
       <c r="BY3" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="BZ3" s="28">
         <v>16.403890000000001</v>
@@ -20693,7 +20688,7 @@
       </c>
       <c r="CB3" s="27"/>
       <c r="CC3" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CD3" s="28">
         <v>15.195111848378099</v>
@@ -20702,7 +20697,7 @@
         <v>2.3762833505952101E-8</v>
       </c>
       <c r="CG3" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CH3" s="28">
         <v>16.602139999999999</v>
@@ -20712,7 +20707,7 @@
       </c>
       <c r="CJ3" s="27"/>
       <c r="CK3" s="28" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="CL3" s="28">
         <v>16.443349999999999</v>
@@ -20722,7 +20717,7 @@
       </c>
       <c r="CN3" s="27"/>
       <c r="CO3" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CP3" s="18">
         <v>6.2046590410000002</v>
@@ -20731,7 +20726,7 @@
         <v>2.4900000000000002E-10</v>
       </c>
       <c r="CS3" s="18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="CT3" s="18">
         <v>6.1074903000000003</v>
@@ -20740,7 +20735,7 @@
         <v>2.50661E-10</v>
       </c>
       <c r="CW3" s="18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="CX3" s="18">
         <v>22.757381259999999</v>
@@ -20749,7 +20744,7 @@
         <v>1.12936E-7</v>
       </c>
       <c r="DA3" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="DB3" s="28">
         <v>8.0650600000000008</v>
@@ -20759,7 +20754,7 @@
       </c>
       <c r="DD3" s="27"/>
       <c r="DE3" s="30" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="DF3" s="28">
         <v>12.33919</v>
@@ -20770,7 +20765,7 @@
     </row>
     <row r="4" spans="1:111" ht="13.8">
       <c r="A4" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B4" s="18">
         <v>14.940431759999999</v>
@@ -20779,7 +20774,7 @@
         <v>2.88E-8</v>
       </c>
       <c r="E4" s="18" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F4" s="18">
         <v>19.068539789999999</v>
@@ -20788,7 +20783,7 @@
         <v>1.88E-8</v>
       </c>
       <c r="I4" s="18" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J4" s="18">
         <v>2.9897238549999998</v>
@@ -20797,7 +20792,7 @@
         <v>1.1000000000000001E-8</v>
       </c>
       <c r="M4" s="18" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="N4" s="18">
         <v>4.9403734659999996</v>
@@ -20807,7 +20802,7 @@
       </c>
       <c r="P4" s="27"/>
       <c r="Q4" s="18" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="R4" s="18">
         <v>6.2705580530000002</v>
@@ -20817,7 +20812,7 @@
       </c>
       <c r="T4" s="27"/>
       <c r="U4" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="V4" s="18">
         <v>9.6160908750369707</v>
@@ -20827,7 +20822,7 @@
       </c>
       <c r="X4" s="27"/>
       <c r="Y4" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="Z4" s="28">
         <v>2.59463</v>
@@ -20837,7 +20832,7 @@
       </c>
       <c r="AB4" s="27"/>
       <c r="AC4" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="AD4" s="28">
         <v>4.7031499999999999</v>
@@ -20847,7 +20842,7 @@
       </c>
       <c r="AF4" s="27"/>
       <c r="AG4" s="18" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="AH4" s="18">
         <v>5.4277567574988197</v>
@@ -20856,7 +20851,7 @@
         <v>9.4881318507116005E-10</v>
       </c>
       <c r="AK4" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AL4" s="28">
         <v>2.4983200000000001</v>
@@ -20866,7 +20861,7 @@
       </c>
       <c r="AN4" s="27"/>
       <c r="AO4" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AP4" s="28">
         <v>3.40022</v>
@@ -20876,7 +20871,7 @@
       </c>
       <c r="AR4" s="27"/>
       <c r="AS4" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="AT4" s="28">
         <v>5.1089486157785897</v>
@@ -20885,7 +20880,7 @@
         <v>7.71394007361839E-10</v>
       </c>
       <c r="AW4" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AX4" s="18">
         <v>16.512356489999998</v>
@@ -20894,7 +20889,7 @@
         <v>1.1200000000000001E-9</v>
       </c>
       <c r="BA4" s="28" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BB4" s="28">
         <v>5.4437199999999999</v>
@@ -20904,7 +20899,7 @@
       </c>
       <c r="BD4" s="27"/>
       <c r="BE4" s="30" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="BF4" s="28">
         <v>7.28165</v>
@@ -20914,7 +20909,7 @@
       </c>
       <c r="BH4" s="27"/>
       <c r="BI4" s="18" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BJ4" s="18">
         <v>13.89258508</v>
@@ -20923,7 +20918,7 @@
         <v>8.4800000000000007E-11</v>
       </c>
       <c r="BM4" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BN4" s="28">
         <v>7.5273300000000001</v>
@@ -20933,7 +20928,7 @@
       </c>
       <c r="BP4" s="27"/>
       <c r="BQ4" s="28" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="BR4" s="28">
         <v>5.0414599999999998</v>
@@ -20943,7 +20938,7 @@
       </c>
       <c r="BT4" s="27"/>
       <c r="BU4" s="18" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="BV4" s="18">
         <v>17.868644</v>
@@ -20952,7 +20947,7 @@
         <v>3.3699999999999997E-8</v>
       </c>
       <c r="BY4" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="BZ4" s="28">
         <v>16.602139999999999</v>
@@ -20962,7 +20957,7 @@
       </c>
       <c r="CB4" s="27"/>
       <c r="CC4" s="28" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="CD4" s="28">
         <v>15.6396894377182</v>
@@ -20971,7 +20966,7 @@
         <v>2.6159341254508799E-8</v>
       </c>
       <c r="CG4" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CH4" s="28">
         <v>17.005849999999999</v>
@@ -20981,7 +20976,7 @@
       </c>
       <c r="CJ4" s="27"/>
       <c r="CK4" s="28" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="CL4" s="28">
         <v>16.802779999999998</v>
@@ -21009,7 +21004,7 @@
         <v>5.1148199999999999E-10</v>
       </c>
       <c r="CW4" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="CX4" s="18">
         <v>22.962772789999999</v>
@@ -21018,7 +21013,7 @@
         <v>1.2571299999999998E-7</v>
       </c>
       <c r="DA4" s="28" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="DB4" s="28">
         <v>9.3412600000000001</v>
@@ -21028,7 +21023,7 @@
       </c>
       <c r="DD4" s="27"/>
       <c r="DE4" s="30" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="DF4" s="28">
         <v>14.51445</v>

</xml_diff>